<commit_message>
Added bootstrap and confidence intervals to risk ratios for job quality
</commit_message>
<xml_diff>
--- a/Results/quality.xlsx
+++ b/Results/quality.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,6 +403,36 @@
           <t>rr_poverty</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>rr_physical_95low</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>rr_stress_95low</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>rr_poverty_95low</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rr_physical_95up</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>rr_stress_95up</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>rr_poverty_95up</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -438,6 +468,24 @@
       <c r="I2">
         <v>1.050483634589852</v>
       </c>
+      <c r="J2">
+        <v>1.01256515795278</v>
+      </c>
+      <c r="K2">
+        <v>1.179248466323973</v>
+      </c>
+      <c r="L2">
+        <v>0.9377009350381036</v>
+      </c>
+      <c r="M2">
+        <v>1.080764217261617</v>
+      </c>
+      <c r="N2">
+        <v>1.30371565439118</v>
+      </c>
+      <c r="O2">
+        <v>1.190528818277899</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -473,6 +521,24 @@
       <c r="I3">
         <v>1.106747649520144</v>
       </c>
+      <c r="J3">
+        <v>1.021397836602722</v>
+      </c>
+      <c r="K3">
+        <v>1.138869411195226</v>
+      </c>
+      <c r="L3">
+        <v>0.9954268387171304</v>
+      </c>
+      <c r="M3">
+        <v>1.094605854342868</v>
+      </c>
+      <c r="N3">
+        <v>1.253797880451045</v>
+      </c>
+      <c r="O3">
+        <v>1.217252763449194</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,6 +574,24 @@
       <c r="I4">
         <v>1.045574404598978</v>
       </c>
+      <c r="J4">
+        <v>1.016995271843494</v>
+      </c>
+      <c r="K4">
+        <v>1.160075802067979</v>
+      </c>
+      <c r="L4">
+        <v>0.9432293953044814</v>
+      </c>
+      <c r="M4">
+        <v>1.103546737346204</v>
+      </c>
+      <c r="N4">
+        <v>1.274389571943006</v>
+      </c>
+      <c r="O4">
+        <v>1.169858813629332</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -543,6 +627,24 @@
       <c r="I5">
         <v>1.098817005782724</v>
       </c>
+      <c r="J5">
+        <v>1.026316720233759</v>
+      </c>
+      <c r="K5">
+        <v>1.139671311281238</v>
+      </c>
+      <c r="L5">
+        <v>0.9957410649959413</v>
+      </c>
+      <c r="M5">
+        <v>1.119083014790386</v>
+      </c>
+      <c r="N5">
+        <v>1.249695165377421</v>
+      </c>
+      <c r="O5">
+        <v>1.206099228626335</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -578,6 +680,24 @@
       <c r="I6">
         <v>1.056943099933577</v>
       </c>
+      <c r="J6">
+        <v>1.0173123267935</v>
+      </c>
+      <c r="K6">
+        <v>1.120546570313376</v>
+      </c>
+      <c r="L6">
+        <v>0.9303853489482627</v>
+      </c>
+      <c r="M6">
+        <v>1.110152924532219</v>
+      </c>
+      <c r="N6">
+        <v>1.211245153329125</v>
+      </c>
+      <c r="O6">
+        <v>1.217050248481755</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -613,6 +733,24 @@
       <c r="I7">
         <v>1.122686879311817</v>
       </c>
+      <c r="J7">
+        <v>1.027355266201154</v>
+      </c>
+      <c r="K7">
+        <v>1.098066442082346</v>
+      </c>
+      <c r="L7">
+        <v>0.9946751112361216</v>
+      </c>
+      <c r="M7">
+        <v>1.124346328721834</v>
+      </c>
+      <c r="N7">
+        <v>1.177147881837192</v>
+      </c>
+      <c r="O7">
+        <v>1.253983410741078</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +786,24 @@
       <c r="I8">
         <v>1.056139266225322</v>
       </c>
+      <c r="J8">
+        <v>1.017736679430296</v>
+      </c>
+      <c r="K8">
+        <v>1.156085726534873</v>
+      </c>
+      <c r="L8">
+        <v>0.9303805917231224</v>
+      </c>
+      <c r="M8">
+        <v>1.113031345557702</v>
+      </c>
+      <c r="N8">
+        <v>1.258940396189938</v>
+      </c>
+      <c r="O8">
+        <v>1.216384643476736</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -683,6 +839,24 @@
       <c r="I9">
         <v>1.120523313161906</v>
       </c>
+      <c r="J9">
+        <v>1.033218559302173</v>
+      </c>
+      <c r="K9">
+        <v>1.12352753471734</v>
+      </c>
+      <c r="L9">
+        <v>0.9948232440375294</v>
+      </c>
+      <c r="M9">
+        <v>1.14617439113762</v>
+      </c>
+      <c r="N9">
+        <v>1.216799309851935</v>
+      </c>
+      <c r="O9">
+        <v>1.24965469312843</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -718,6 +892,24 @@
       <c r="I10">
         <v>1.05442242154026</v>
       </c>
+      <c r="J10">
+        <v>1.020749171424505</v>
+      </c>
+      <c r="K10">
+        <v>1.136365628382892</v>
+      </c>
+      <c r="L10">
+        <v>0.9329146872228757</v>
+      </c>
+      <c r="M10">
+        <v>1.129732230321504</v>
+      </c>
+      <c r="N10">
+        <v>1.227291662469943</v>
+      </c>
+      <c r="O10">
+        <v>1.208828122826497</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -753,6 +945,24 @@
       <c r="I11">
         <v>1.118150736159423</v>
       </c>
+      <c r="J11">
+        <v>1.036123910653293</v>
+      </c>
+      <c r="K11">
+        <v>1.123602155300152</v>
+      </c>
+      <c r="L11">
+        <v>0.9949415867868214</v>
+      </c>
+      <c r="M11">
+        <v>1.163601779074461</v>
+      </c>
+      <c r="N11">
+        <v>1.217905858740534</v>
+      </c>
+      <c r="O11">
+        <v>1.243724626160237</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -788,6 +998,24 @@
       <c r="I12">
         <v>1.05956248074361</v>
       </c>
+      <c r="J12">
+        <v>1.023403753044698</v>
+      </c>
+      <c r="K12">
+        <v>1.114250915312967</v>
+      </c>
+      <c r="L12">
+        <v>0.9270682107036017</v>
+      </c>
+      <c r="M12">
+        <v>1.145114500369772</v>
+      </c>
+      <c r="N12">
+        <v>1.188547661986049</v>
+      </c>
+      <c r="O12">
+        <v>1.228293644953695</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -823,6 +1051,24 @@
       <c r="I13">
         <v>1.129839062148083</v>
       </c>
+      <c r="J13">
+        <v>1.040234584110352</v>
+      </c>
+      <c r="K13">
+        <v>1.096757012981129</v>
+      </c>
+      <c r="L13">
+        <v>0.9944408472738675</v>
+      </c>
+      <c r="M13">
+        <v>1.18063482054866</v>
+      </c>
+      <c r="N13">
+        <v>1.168711053250433</v>
+      </c>
+      <c r="O13">
+        <v>1.267724618777162</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -858,6 +1104,24 @@
       <c r="I14">
         <v>1.059093269015841</v>
       </c>
+      <c r="J14">
+        <v>1.031093895965812</v>
+      </c>
+      <c r="K14">
+        <v>1.120449468867102</v>
+      </c>
+      <c r="L14">
+        <v>0.9279574120239251</v>
+      </c>
+      <c r="M14">
+        <v>1.194587325713757</v>
+      </c>
+      <c r="N14">
+        <v>1.197876866690254</v>
+      </c>
+      <c r="O14">
+        <v>1.226603536185932</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -893,6 +1157,24 @@
       <c r="I15">
         <v>1.12994412284401</v>
       </c>
+      <c r="J15">
+        <v>1.045447322304079</v>
+      </c>
+      <c r="K15">
+        <v>1.091864507611691</v>
+      </c>
+      <c r="L15">
+        <v>0.994423042187409</v>
+      </c>
+      <c r="M15">
+        <v>1.205024432247845</v>
+      </c>
+      <c r="N15">
+        <v>1.157843775384524</v>
+      </c>
+      <c r="O15">
+        <v>1.267317158983811</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -928,6 +1210,24 @@
       <c r="I16">
         <v>1.05639414197546</v>
       </c>
+      <c r="J16">
+        <v>1.026774823330058</v>
+      </c>
+      <c r="K16">
+        <v>1.109460273814597</v>
+      </c>
+      <c r="L16">
+        <v>0.9312197572538751</v>
+      </c>
+      <c r="M16">
+        <v>1.174751794305749</v>
+      </c>
+      <c r="N16">
+        <v>1.194865927990239</v>
+      </c>
+      <c r="O16">
+        <v>1.214911339040698</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -963,6 +1263,24 @@
       <c r="I17">
         <v>1.125287773663258</v>
       </c>
+      <c r="J17">
+        <v>1.040536347952977</v>
+      </c>
+      <c r="K17">
+        <v>1.098843498333451</v>
+      </c>
+      <c r="L17">
+        <v>0.9946209566745439</v>
+      </c>
+      <c r="M17">
+        <v>1.180640130864909</v>
+      </c>
+      <c r="N17">
+        <v>1.182667975858652</v>
+      </c>
+      <c r="O17">
+        <v>1.258248855876363</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -998,6 +1316,24 @@
       <c r="I18">
         <v>1.060457427763088</v>
       </c>
+      <c r="J18">
+        <v>1.03320098100771</v>
+      </c>
+      <c r="K18">
+        <v>1.091435160835794</v>
+      </c>
+      <c r="L18">
+        <v>0.9259802667476098</v>
+      </c>
+      <c r="M18">
+        <v>1.209345418056715</v>
+      </c>
+      <c r="N18">
+        <v>1.149304905756631</v>
+      </c>
+      <c r="O18">
+        <v>1.232243413256689</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1032,6 +1368,24 @@
       </c>
       <c r="I19">
         <v>1.132914905882109</v>
+      </c>
+      <c r="J19">
+        <v>1.048790066386728</v>
+      </c>
+      <c r="K19">
+        <v>1.075379423427375</v>
+      </c>
+      <c r="L19">
+        <v>0.9943239381972824</v>
+      </c>
+      <c r="M19">
+        <v>1.223255167240542</v>
+      </c>
+      <c r="N19">
+        <v>1.12743979681619</v>
+      </c>
+      <c r="O19">
+        <v>1.273555561072473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results on experiencing any of the three types of low quality
</commit_message>
<xml_diff>
--- a/Results/quality.xlsx
+++ b/Results/quality.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,47 +390,67 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>anybad</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>rr_physical</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>rr_stress</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>rr_poverty</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>rr_anybad</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>rr_physical_95low</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>rr_stress_95low</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>rr_poverty_95low</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>rr_anybad_95low</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>rr_physical_95up</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>rr_stress_95up</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>rr_poverty_95up</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rr_anybad_95up</t>
         </is>
       </c>
     </row>
@@ -460,31 +480,43 @@
         <v>0.1718435557107438</v>
       </c>
       <c r="G2">
+        <v>0.8175230068533549</v>
+      </c>
+      <c r="H2">
         <v>1.044098255695232</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.237123360808975</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1.050483634589852</v>
       </c>
-      <c r="J2">
-        <v>1.01256515795278</v>
-      </c>
       <c r="K2">
-        <v>1.179248466323973</v>
+        <v>1.053956506267101</v>
       </c>
       <c r="L2">
-        <v>0.9377009350381036</v>
+        <v>1.013214108030252</v>
       </c>
       <c r="M2">
-        <v>1.080764217261617</v>
+        <v>1.177261567584297</v>
       </c>
       <c r="N2">
-        <v>1.30371565439118</v>
+        <v>0.9393582234967901</v>
       </c>
       <c r="O2">
-        <v>1.190528818277899</v>
+        <v>1.032635334999701</v>
+      </c>
+      <c r="P2">
+        <v>1.080641699909626</v>
+      </c>
+      <c r="Q2">
+        <v>1.308272987123011</v>
+      </c>
+      <c r="R2">
+        <v>1.177921432600948</v>
+      </c>
+      <c r="S2">
+        <v>1.080691074729922</v>
       </c>
     </row>
     <row r="3">
@@ -513,31 +545,43 @@
         <v>0.2040440544126476</v>
       </c>
       <c r="G3">
+        <v>0.8386909240581151</v>
+      </c>
+      <c r="H3">
         <v>1.054004392494821</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1.193829524087098</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1.106747649520144</v>
       </c>
-      <c r="J3">
-        <v>1.021397836602722</v>
-      </c>
       <c r="K3">
-        <v>1.138869411195226</v>
+        <v>1.05346833756508</v>
       </c>
       <c r="L3">
-        <v>0.9954268387171304</v>
+        <v>1.021972262622803</v>
       </c>
       <c r="M3">
-        <v>1.094605854342868</v>
+        <v>1.146143366440801</v>
       </c>
       <c r="N3">
-        <v>1.253797880451045</v>
+        <v>1.0015820107145</v>
       </c>
       <c r="O3">
-        <v>1.217252763449194</v>
+        <v>1.035052565250807</v>
+      </c>
+      <c r="P3">
+        <v>1.090851643787171</v>
+      </c>
+      <c r="Q3">
+        <v>1.250298774655401</v>
+      </c>
+      <c r="R3">
+        <v>1.214972318295113</v>
+      </c>
+      <c r="S3">
+        <v>1.077299313986833</v>
       </c>
     </row>
     <row r="4">
@@ -566,31 +610,43 @@
         <v>0.2523767916092918</v>
       </c>
       <c r="G4">
+        <v>0.8193264327177946</v>
+      </c>
+      <c r="H4">
         <v>1.058382813377533</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.211358862466423</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.045574404598978</v>
       </c>
-      <c r="J4">
-        <v>1.016995271843494</v>
-      </c>
       <c r="K4">
-        <v>1.160075802067979</v>
+        <v>1.05342325241806</v>
       </c>
       <c r="L4">
-        <v>0.9432293953044814</v>
+        <v>1.016730250379123</v>
       </c>
       <c r="M4">
-        <v>1.103546737346204</v>
+        <v>1.158456093903216</v>
       </c>
       <c r="N4">
-        <v>1.274389571943006</v>
+        <v>0.9450488182099978</v>
       </c>
       <c r="O4">
-        <v>1.169858813629332</v>
+        <v>1.032529503223918</v>
+      </c>
+      <c r="P4">
+        <v>1.103426121425787</v>
+      </c>
+      <c r="Q4">
+        <v>1.272277271588753</v>
+      </c>
+      <c r="R4">
+        <v>1.158013837665733</v>
+      </c>
+      <c r="S4">
+        <v>1.076964136236134</v>
       </c>
     </row>
     <row r="5">
@@ -619,31 +675,43 @@
         <v>0.263178312295711</v>
       </c>
       <c r="G5">
+        <v>0.8369997955036165</v>
+      </c>
+      <c r="H5">
         <v>1.069159225410057</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.19401426989448</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1.098817005782724</v>
       </c>
-      <c r="J5">
-        <v>1.026316720233759</v>
-      </c>
       <c r="K5">
-        <v>1.139671311281238</v>
+        <v>1.054028887750431</v>
       </c>
       <c r="L5">
-        <v>0.9957410649959413</v>
+        <v>1.027933323073099</v>
       </c>
       <c r="M5">
-        <v>1.119083014790386</v>
+        <v>1.146196841934884</v>
       </c>
       <c r="N5">
-        <v>1.249695165377421</v>
+        <v>1.001467766537552</v>
       </c>
       <c r="O5">
-        <v>1.206099228626335</v>
+        <v>1.036108510667731</v>
+      </c>
+      <c r="P5">
+        <v>1.112353739243522</v>
+      </c>
+      <c r="Q5">
+        <v>1.249971289715862</v>
+      </c>
+      <c r="R5">
+        <v>1.201077429356429</v>
+      </c>
+      <c r="S5">
+        <v>1.074023842891252</v>
       </c>
     </row>
     <row r="6">
@@ -672,31 +740,43 @@
         <v>0.06587955580206835</v>
       </c>
       <c r="G6">
+        <v>0.8268440813116509</v>
+      </c>
+      <c r="H6">
         <v>1.060409947850499</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1.161259776203038</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1.056943099933577</v>
       </c>
-      <c r="J6">
-        <v>1.0173123267935</v>
-      </c>
       <c r="K6">
-        <v>1.120546570313376</v>
+        <v>1.051200363677547</v>
       </c>
       <c r="L6">
-        <v>0.9303853489482627</v>
+        <v>1.017066322711784</v>
       </c>
       <c r="M6">
-        <v>1.110152924532219</v>
+        <v>1.117767919908355</v>
       </c>
       <c r="N6">
-        <v>1.211245153329125</v>
+        <v>0.9305699109706342</v>
       </c>
       <c r="O6">
-        <v>1.217050248481755</v>
+        <v>1.031149756242346</v>
+      </c>
+      <c r="P6">
+        <v>1.107693991981422</v>
+      </c>
+      <c r="Q6">
+        <v>1.207719926536266</v>
+      </c>
+      <c r="R6">
+        <v>1.207015715922681</v>
+      </c>
+      <c r="S6">
+        <v>1.075558763509092</v>
       </c>
     </row>
     <row r="7">
@@ -725,31 +805,43 @@
         <v>0.08519436753152562</v>
       </c>
       <c r="G7">
+        <v>0.8398475075689038</v>
+      </c>
+      <c r="H7">
         <v>1.072862908953344</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.137085132776632</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1.122686879311817</v>
       </c>
-      <c r="J7">
-        <v>1.027355266201154</v>
-      </c>
       <c r="K7">
-        <v>1.098066442082346</v>
+        <v>1.053084970434521</v>
       </c>
       <c r="L7">
-        <v>0.9946751112361216</v>
+        <v>1.029044207173212</v>
       </c>
       <c r="M7">
-        <v>1.124346328721834</v>
+        <v>1.102392628159572</v>
       </c>
       <c r="N7">
-        <v>1.177147881837192</v>
+        <v>1.001829012983137</v>
       </c>
       <c r="O7">
-        <v>1.253983410741078</v>
+        <v>1.035097045268287</v>
+      </c>
+      <c r="P7">
+        <v>1.120741644427255</v>
+      </c>
+      <c r="Q7">
+        <v>1.177113732523665</v>
+      </c>
+      <c r="R7">
+        <v>1.25171213644987</v>
+      </c>
+      <c r="S7">
+        <v>1.075633723840007</v>
       </c>
     </row>
     <row r="8">
@@ -778,31 +870,43 @@
         <v>0.07906600862062732</v>
       </c>
       <c r="G8">
+        <v>0.7686456608164728</v>
+      </c>
+      <c r="H8">
         <v>1.064504197049108</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1.201974245403202</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.056139266225322</v>
       </c>
-      <c r="J8">
-        <v>1.017736679430296</v>
-      </c>
       <c r="K8">
-        <v>1.156085726534873</v>
+        <v>1.068409017689398</v>
       </c>
       <c r="L8">
-        <v>0.9303805917231224</v>
+        <v>1.019350671261173</v>
       </c>
       <c r="M8">
-        <v>1.113031345557702</v>
+        <v>1.150516758427119</v>
       </c>
       <c r="N8">
-        <v>1.258940396189938</v>
+        <v>0.9320771727041821</v>
       </c>
       <c r="O8">
-        <v>1.216384643476736</v>
+        <v>1.043327013531331</v>
+      </c>
+      <c r="P8">
+        <v>1.110405551463595</v>
+      </c>
+      <c r="Q8">
+        <v>1.260815716801262</v>
+      </c>
+      <c r="R8">
+        <v>1.20311753225668</v>
+      </c>
+      <c r="S8">
+        <v>1.09744546864995</v>
       </c>
     </row>
     <row r="9">
@@ -831,31 +935,43 @@
         <v>0.1013268383487709</v>
       </c>
       <c r="G9">
+        <v>0.7679803848535932</v>
+      </c>
+      <c r="H9">
         <v>1.086727703560965</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1.169755052274979</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.120523313161906</v>
       </c>
-      <c r="J9">
-        <v>1.033218559302173</v>
-      </c>
       <c r="K9">
-        <v>1.12352753471734</v>
+        <v>1.076906417273369</v>
       </c>
       <c r="L9">
-        <v>0.9948232440375294</v>
+        <v>1.035001138198733</v>
       </c>
       <c r="M9">
-        <v>1.14617439113762</v>
+        <v>1.129628157823973</v>
       </c>
       <c r="N9">
-        <v>1.216799309851935</v>
+        <v>1.001784824149812</v>
       </c>
       <c r="O9">
-        <v>1.24965469312843</v>
+        <v>1.051708400033905</v>
+      </c>
+      <c r="P9">
+        <v>1.143951573749473</v>
+      </c>
+      <c r="Q9">
+        <v>1.218419535632835</v>
+      </c>
+      <c r="R9">
+        <v>1.245031906178167</v>
+      </c>
+      <c r="S9">
+        <v>1.103342044859157</v>
       </c>
     </row>
     <row r="10">
@@ -884,31 +1000,43 @@
         <v>0.1072299077005703</v>
       </c>
       <c r="G10">
+        <v>0.7784494204094269</v>
+      </c>
+      <c r="H10">
         <v>1.074349537467539</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1.177110981494486</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1.05442242154026</v>
       </c>
-      <c r="J10">
-        <v>1.020749171424505</v>
-      </c>
       <c r="K10">
-        <v>1.136365628382892</v>
+        <v>1.065510150238786</v>
       </c>
       <c r="L10">
-        <v>0.9329146872228757</v>
+        <v>1.021298947293009</v>
       </c>
       <c r="M10">
-        <v>1.129732230321504</v>
+        <v>1.132783373620724</v>
       </c>
       <c r="N10">
-        <v>1.227291662469943</v>
+        <v>0.9341703872701977</v>
       </c>
       <c r="O10">
-        <v>1.208828122826497</v>
+        <v>1.042270096761871</v>
+      </c>
+      <c r="P10">
+        <v>1.130754085254148</v>
+      </c>
+      <c r="Q10">
+        <v>1.229568451598431</v>
+      </c>
+      <c r="R10">
+        <v>1.196362850826908</v>
+      </c>
+      <c r="S10">
+        <v>1.092956980082138</v>
       </c>
     </row>
     <row r="11">
@@ -937,31 +1065,43 @@
         <v>0.1190177831141052</v>
       </c>
       <c r="G11">
+        <v>0.7735265738580027</v>
+      </c>
+      <c r="H11">
         <v>1.096142850300793</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1.170936579646361</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1.118150736159423</v>
       </c>
-      <c r="J11">
-        <v>1.036123910653293</v>
-      </c>
       <c r="K11">
-        <v>1.123602155300152</v>
+        <v>1.075068048885502</v>
       </c>
       <c r="L11">
-        <v>0.9949415867868214</v>
+        <v>1.038417612170542</v>
       </c>
       <c r="M11">
-        <v>1.163601779074461</v>
+        <v>1.128334827182179</v>
       </c>
       <c r="N11">
-        <v>1.217905858740534</v>
+        <v>1.001744630190954</v>
       </c>
       <c r="O11">
-        <v>1.243724626160237</v>
+        <v>1.051408116696234</v>
+      </c>
+      <c r="P11">
+        <v>1.156090774583735</v>
+      </c>
+      <c r="Q11">
+        <v>1.223374416771505</v>
+      </c>
+      <c r="R11">
+        <v>1.240218270360443</v>
+      </c>
+      <c r="S11">
+        <v>1.10412702004948</v>
       </c>
     </row>
     <row r="12">
@@ -990,31 +1130,43 @@
         <v>0.02291004468227386</v>
       </c>
       <c r="G12">
+        <v>0.7782213785350327</v>
+      </c>
+      <c r="H12">
         <v>1.082125677360067</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1.148395490054291</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1.05956248074361</v>
       </c>
-      <c r="J12">
-        <v>1.023403753044698</v>
-      </c>
       <c r="K12">
-        <v>1.114250915312967</v>
+        <v>1.065577579795864</v>
       </c>
       <c r="L12">
-        <v>0.9270682107036017</v>
+        <v>1.023281762176376</v>
       </c>
       <c r="M12">
-        <v>1.145114500369772</v>
+        <v>1.11136246562521</v>
       </c>
       <c r="N12">
-        <v>1.188547661986049</v>
+        <v>0.9279531562222474</v>
       </c>
       <c r="O12">
-        <v>1.228293644953695</v>
+        <v>1.041697088410233</v>
+      </c>
+      <c r="P12">
+        <v>1.143563474572525</v>
+      </c>
+      <c r="Q12">
+        <v>1.192031752212329</v>
+      </c>
+      <c r="R12">
+        <v>1.216672860596275</v>
+      </c>
+      <c r="S12">
+        <v>1.092734432266782</v>
       </c>
     </row>
     <row r="13">
@@ -1043,31 +1195,43 @@
         <v>0.03186464572458923</v>
       </c>
       <c r="G13">
+        <v>0.7678835954183992</v>
+      </c>
+      <c r="H13">
         <v>1.105665731865027</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>1.133812776795585</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1.129839062148083</v>
       </c>
-      <c r="J13">
-        <v>1.040234584110352</v>
-      </c>
       <c r="K13">
-        <v>1.096757012981129</v>
+        <v>1.076938499598331</v>
       </c>
       <c r="L13">
-        <v>0.9944408472738675</v>
+        <v>1.04320478350242</v>
       </c>
       <c r="M13">
-        <v>1.18063482054866</v>
+        <v>1.102747176908807</v>
       </c>
       <c r="N13">
-        <v>1.168711053250433</v>
+        <v>1.001918740400947</v>
       </c>
       <c r="O13">
-        <v>1.267724618777162</v>
+        <v>1.053282848891016</v>
+      </c>
+      <c r="P13">
+        <v>1.173172326714252</v>
+      </c>
+      <c r="Q13">
+        <v>1.170634527022718</v>
+      </c>
+      <c r="R13">
+        <v>1.263791016657192</v>
+      </c>
+      <c r="S13">
+        <v>1.103020414838134</v>
       </c>
     </row>
     <row r="14">
@@ -1096,31 +1260,43 @@
         <v>0.03060720672784347</v>
       </c>
       <c r="G14">
+        <v>0.705501664307754</v>
+      </c>
+      <c r="H14">
         <v>1.110297834755405</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>1.155644161590905</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1.059093269015841</v>
       </c>
-      <c r="J14">
-        <v>1.031093895965812</v>
-      </c>
       <c r="K14">
-        <v>1.120449468867102</v>
+        <v>1.08708002593324</v>
       </c>
       <c r="L14">
-        <v>0.9279574120239251</v>
+        <v>1.032028395153306</v>
       </c>
       <c r="M14">
-        <v>1.194587325713757</v>
+        <v>1.116487137873932</v>
       </c>
       <c r="N14">
-        <v>1.197876866690254</v>
+        <v>0.9286757853284469</v>
       </c>
       <c r="O14">
-        <v>1.226603536185932</v>
+        <v>1.055772744729348</v>
+      </c>
+      <c r="P14">
+        <v>1.194189475733554</v>
+      </c>
+      <c r="Q14">
+        <v>1.203620956084896</v>
+      </c>
+      <c r="R14">
+        <v>1.214669099716139</v>
+      </c>
+      <c r="S14">
+        <v>1.124642813695595</v>
       </c>
     </row>
     <row r="15">
@@ -1149,31 +1325,43 @@
         <v>0.0310812684235801</v>
       </c>
       <c r="G15">
+        <v>0.7392574504319697</v>
+      </c>
+      <c r="H15">
         <v>1.120484927432569</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1.12390602488182</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1.12994412284401</v>
       </c>
-      <c r="J15">
-        <v>1.045447322304079</v>
-      </c>
       <c r="K15">
-        <v>1.091864507611691</v>
+        <v>1.086427069130977</v>
       </c>
       <c r="L15">
-        <v>0.994423042187409</v>
+        <v>1.049752996338377</v>
       </c>
       <c r="M15">
-        <v>1.205024432247845</v>
+        <v>1.092596943074343</v>
       </c>
       <c r="N15">
-        <v>1.157843775384524</v>
+        <v>1.001921930265669</v>
       </c>
       <c r="O15">
-        <v>1.267317158983811</v>
+        <v>1.058579656712467</v>
+      </c>
+      <c r="P15">
+        <v>1.199021002126987</v>
+      </c>
+      <c r="Q15">
+        <v>1.161494096996591</v>
+      </c>
+      <c r="R15">
+        <v>1.262459936810329</v>
+      </c>
+      <c r="S15">
+        <v>1.11816940764967</v>
       </c>
     </row>
     <row r="16">
@@ -1202,31 +1390,43 @@
         <v>0.07488491118805768</v>
       </c>
       <c r="G16">
+        <v>0.7491129596126874</v>
+      </c>
+      <c r="H16">
         <v>1.099664863840935</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>1.148532833266064</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1.05639414197546</v>
       </c>
-      <c r="J16">
-        <v>1.026774823330058</v>
-      </c>
       <c r="K16">
-        <v>1.109460273814597</v>
+        <v>1.074184629708982</v>
       </c>
       <c r="L16">
-        <v>0.9312197572538751</v>
+        <v>1.027238502104199</v>
       </c>
       <c r="M16">
-        <v>1.174751794305749</v>
+        <v>1.109570089706756</v>
       </c>
       <c r="N16">
-        <v>1.194865927990239</v>
+        <v>0.9323585693685164</v>
       </c>
       <c r="O16">
-        <v>1.214911339040698</v>
+        <v>1.045488445675182</v>
+      </c>
+      <c r="P16">
+        <v>1.176537087374862</v>
+      </c>
+      <c r="Q16">
+        <v>1.197868008031604</v>
+      </c>
+      <c r="R16">
+        <v>1.199512780459306</v>
+      </c>
+      <c r="S16">
+        <v>1.110147578992588</v>
       </c>
     </row>
     <row r="17">
@@ -1255,31 +1455,43 @@
         <v>0.06580099135715321</v>
       </c>
       <c r="G17">
+        <v>0.7751774536136742</v>
+      </c>
+      <c r="H17">
         <v>1.106174303322158</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>1.139799305085285</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>1.125287773663258</v>
       </c>
-      <c r="J17">
-        <v>1.040536347952977</v>
-      </c>
       <c r="K17">
-        <v>1.098843498333451</v>
+        <v>1.074520839774421</v>
       </c>
       <c r="L17">
-        <v>0.9946209566745439</v>
+        <v>1.044191218642741</v>
       </c>
       <c r="M17">
-        <v>1.180640130864909</v>
+        <v>1.10149487311788</v>
       </c>
       <c r="N17">
-        <v>1.182667975858652</v>
+        <v>1.001861028740489</v>
       </c>
       <c r="O17">
-        <v>1.258248855876363</v>
+        <v>1.048967267030918</v>
+      </c>
+      <c r="P17">
+        <v>1.175625242699108</v>
+      </c>
+      <c r="Q17">
+        <v>1.186480890678051</v>
+      </c>
+      <c r="R17">
+        <v>1.255158002195386</v>
+      </c>
+      <c r="S17">
+        <v>1.110336569341654</v>
       </c>
     </row>
     <row r="18">
@@ -1308,31 +1520,43 @@
         <v>0.008228927771815584</v>
       </c>
       <c r="G18">
+        <v>0.7507024640566946</v>
+      </c>
+      <c r="H18">
         <v>1.118240713509426</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>1.117002258861124</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.060457427763088</v>
       </c>
-      <c r="J18">
-        <v>1.03320098100771</v>
-      </c>
       <c r="K18">
-        <v>1.091435160835794</v>
+        <v>1.073714630148952</v>
       </c>
       <c r="L18">
-        <v>0.9259802667476098</v>
+        <v>1.033145783033963</v>
       </c>
       <c r="M18">
-        <v>1.209345418056715</v>
+        <v>1.088587579263204</v>
       </c>
       <c r="N18">
-        <v>1.149304905756631</v>
+        <v>0.9269355032269437</v>
       </c>
       <c r="O18">
-        <v>1.232243413256689</v>
+        <v>1.047706556614987</v>
+      </c>
+      <c r="P18">
+        <v>1.207720122488238</v>
+      </c>
+      <c r="Q18">
+        <v>1.151406130392854</v>
+      </c>
+      <c r="R18">
+        <v>1.219519675521085</v>
+      </c>
+      <c r="S18">
+        <v>1.103358078668907</v>
       </c>
     </row>
     <row r="19">
@@ -1361,31 +1585,43 @@
         <v>0.008929844641825516</v>
       </c>
       <c r="G19">
+        <v>0.7712961313750915</v>
+      </c>
+      <c r="H19">
         <v>1.130363315869883</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>1.101589580515479</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>1.132914905882109</v>
       </c>
-      <c r="J19">
-        <v>1.048790066386728</v>
-      </c>
       <c r="K19">
-        <v>1.075379423427375</v>
+        <v>1.075807362844742</v>
       </c>
       <c r="L19">
-        <v>0.9943239381972824</v>
+        <v>1.052815520546763</v>
       </c>
       <c r="M19">
-        <v>1.223255167240542</v>
+        <v>1.077949976174376</v>
       </c>
       <c r="N19">
-        <v>1.12743979681619</v>
+        <v>1.001960602022187</v>
       </c>
       <c r="O19">
-        <v>1.273555561072473</v>
+        <v>1.051911592115921</v>
+      </c>
+      <c r="P19">
+        <v>1.216269105300662</v>
+      </c>
+      <c r="Q19">
+        <v>1.128794505774226</v>
+      </c>
+      <c r="R19">
+        <v>1.270580219275513</v>
+      </c>
+      <c r="S19">
+        <v>1.102033319354732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>